<commit_message>
add a method to find the optimal maxlag
</commit_message>
<xml_diff>
--- a/Data_Analysis_Temp.xlsx
+++ b/Data_Analysis_Temp.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/yt15482_bristol_ac_uk/Documents/MSc project/Project/Causal_Relationship_Inferring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="114_{9C27FFA0-BA70-47CE-8FAA-F5A9929EE129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24A24113-56A9-46FD-AE92-C2EC46E94F3C}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="114_{9C27FFA0-BA70-47CE-8FAA-F5A9929EE129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E4D2E40-3728-4464-A9FE-3DFB55C47516}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3570" yWindow="270" windowWidth="24465" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="135" windowWidth="21615" windowHeight="15330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="temp" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="3" r:id="rId1"/>
+    <sheet name="3" sheetId="1" r:id="rId2"/>
+    <sheet name="3_Chain" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="16">
   <si>
     <t>SF_F</t>
   </si>
@@ -74,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +88,14 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -164,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -175,6 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -476,19 +487,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCC13CC-3E16-4420-92AF-0E1DB1539B1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +547,7 @@
       <c r="AG1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41">
       <c r="A2" s="1">
         <v>151.28861370000001</v>
       </c>
@@ -556,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41">
       <c r="A3">
         <v>18.144872548173481</v>
       </c>
@@ -588,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41">
       <c r="A4">
         <v>13.043167739999999</v>
       </c>
@@ -620,7 +643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41">
       <c r="A5">
         <v>102.4724198</v>
       </c>
@@ -652,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41">
       <c r="A6">
         <v>87.252722314615113</v>
       </c>
@@ -684,7 +707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41">
       <c r="A7">
         <v>142.16694530000001</v>
       </c>
@@ -716,7 +739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41">
       <c r="A8">
         <v>144.34744670000001</v>
       </c>
@@ -748,7 +771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41">
       <c r="A9">
         <v>118.6129834</v>
       </c>
@@ -780,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41">
       <c r="A10">
         <v>547.7377477</v>
       </c>
@@ -812,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41">
       <c r="A11" s="1">
         <v>237.039198</v>
       </c>
@@ -844,7 +867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41">
       <c r="A12">
         <v>99.352314668538853</v>
       </c>
@@ -876,7 +899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41">
       <c r="A13">
         <v>152.17789880000001</v>
       </c>
@@ -908,7 +931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41">
       <c r="A14">
         <v>137.49003099999999</v>
       </c>
@@ -940,7 +963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41">
       <c r="A15">
         <v>103.9320389460302</v>
       </c>
@@ -972,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41">
       <c r="A16">
         <v>194.05169040000001</v>
       </c>
@@ -1004,7 +1027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>123.3880415</v>
       </c>
@@ -1036,7 +1059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>184.47241629999999</v>
       </c>
@@ -1068,7 +1091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>177.11347960000001</v>
       </c>
@@ -1100,7 +1123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="3">
         <v>5.8226256999999997E-2</v>
       </c>
@@ -1132,7 +1155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="5">
         <v>9.5424012542198291</v>
       </c>
@@ -1164,7 +1187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>18.333439259999999</v>
       </c>
@@ -1196,7 +1219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>1.266682074</v>
       </c>
@@ -1228,7 +1251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="5">
         <v>2.1488472311552119E-2</v>
       </c>
@@ -1260,7 +1283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>4.453177954</v>
       </c>
@@ -1292,7 +1315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>5.1923814999999998E-2</v>
       </c>
@@ -1324,7 +1347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>35.615448110000003</v>
       </c>
@@ -1356,7 +1379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>13.15031301</v>
       </c>
@@ -1388,7 +1411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>2.3085774809999999</v>
       </c>
@@ -1420,7 +1443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="5">
         <v>10.062589490724751</v>
       </c>
@@ -1452,7 +1475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>14.16677833</v>
       </c>
@@ -1484,7 +1507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>1.602727781</v>
       </c>
@@ -1516,7 +1539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="5">
         <v>1.7980002501539209E-3</v>
       </c>
@@ -1548,7 +1571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>4.6749920319999996</v>
       </c>
@@ -1580,7 +1603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>0.79142182000000005</v>
       </c>
@@ -1612,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2">
         <v>43.33895879</v>
       </c>
@@ -1644,7 +1667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="7">
         <v>22.994438290000002</v>
       </c>
@@ -1676,7 +1699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>257.26077809999998</v>
       </c>
@@ -1708,7 +1731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>91.144802719774944</v>
       </c>
@@ -1740,7 +1763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>147.5760951</v>
       </c>
@@ -1772,7 +1795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>138.4628218</v>
       </c>
@@ -1804,7 +1827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>105.8475650499456</v>
       </c>
@@ -1836,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>131.57095129999999</v>
       </c>
@@ -1868,7 +1891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>85.365875020000004</v>
       </c>
@@ -1900,7 +1923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>218.17096040000001</v>
       </c>
@@ -1932,7 +1955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>189.40659120000001</v>
       </c>
@@ -1964,7 +1987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>183.80763669999999</v>
       </c>
@@ -1996,7 +2019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>24.103279169057078</v>
       </c>
@@ -2028,7 +2051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>19.562722969999999</v>
       </c>
@@ -2060,7 +2083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>125.51870510000001</v>
       </c>
@@ -2092,7 +2115,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>88.987891907441011</v>
       </c>
@@ -2124,7 +2147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>108.6605283</v>
       </c>
@@ -2156,7 +2179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>123.4747383</v>
       </c>
@@ -2188,7 +2211,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>131.85811169999999</v>
       </c>
@@ -2220,7 +2243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>443.56007410000001</v>
       </c>
@@ -2256,4 +2279,1780 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025812C9-0D62-47BD-A5D9-414E572E2828}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>490.97772112410911</v>
+      </c>
+      <c r="B2">
+        <v>4.3366021486176927E-87</v>
+      </c>
+      <c r="C2">
+        <v>492.62161974394428</v>
+      </c>
+      <c r="D2">
+        <v>3.8316038272261259E-109</v>
+      </c>
+      <c r="E2">
+        <v>392.81080817298789</v>
+      </c>
+      <c r="F2">
+        <v>2.022863036929462E-87</v>
+      </c>
+      <c r="G2">
+        <v>490.97772112410939</v>
+      </c>
+      <c r="H2">
+        <v>4.3366021486174463E-87</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>425.68300943052441</v>
+      </c>
+      <c r="B3">
+        <v>4.2971041830639383E-76</v>
+      </c>
+      <c r="C3">
+        <v>427.28734238063942</v>
+      </c>
+      <c r="D3">
+        <v>6.3285182408864257E-95</v>
+      </c>
+      <c r="E3">
+        <v>342.28002820419351</v>
+      </c>
+      <c r="F3">
+        <v>2.0338823763951299E-76</v>
+      </c>
+      <c r="G3">
+        <v>425.68300943052509</v>
+      </c>
+      <c r="H3">
+        <v>4.2971041830630823E-76</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>376.45841782820719</v>
+      </c>
+      <c r="B4">
+        <v>2.302940998163475E-67</v>
+      </c>
+      <c r="C4">
+        <v>378.08108342229428</v>
+      </c>
+      <c r="D4">
+        <v>3.2564340211100862E-84</v>
+      </c>
+      <c r="E4">
+        <v>302.21909370380308</v>
+      </c>
+      <c r="F4">
+        <v>1.0822097201134E-67</v>
+      </c>
+      <c r="G4">
+        <v>376.45841782820781</v>
+      </c>
+      <c r="H4">
+        <v>2.3029409981632131E-67</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>336.74751420090371</v>
+      </c>
+      <c r="B5">
+        <v>5.8583066461127468E-60</v>
+      </c>
+      <c r="C5">
+        <v>338.44255202406271</v>
+      </c>
+      <c r="D5">
+        <v>1.3933406800025801E-75</v>
+      </c>
+      <c r="E5">
+        <v>268.28843412632159</v>
+      </c>
+      <c r="F5">
+        <v>2.6788098716104732E-60</v>
+      </c>
+      <c r="G5">
+        <v>336.74751420090462</v>
+      </c>
+      <c r="H5">
+        <v>5.8583066461109151E-60</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>256.89280895584278</v>
+      </c>
+      <c r="B6">
+        <v>6.8460155063133089E-47</v>
+      </c>
+      <c r="C6">
+        <v>258.44659610678542</v>
+      </c>
+      <c r="D6">
+        <v>3.742182167581103E-58</v>
+      </c>
+      <c r="E6">
+        <v>208.25612253988771</v>
+      </c>
+      <c r="F6">
+        <v>3.2986620617364532E-47</v>
+      </c>
+      <c r="G6">
+        <v>256.8928089558417</v>
+      </c>
+      <c r="H6">
+        <v>6.846015506315838E-47</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>220.594323404465</v>
+      </c>
+      <c r="B7">
+        <v>5.5953202920354287E-40</v>
+      </c>
+      <c r="C7">
+        <v>222.2654925211655</v>
+      </c>
+      <c r="D7">
+        <v>2.898899376265785E-50</v>
+      </c>
+      <c r="E7">
+        <v>176.6760420500741</v>
+      </c>
+      <c r="F7">
+        <v>2.5775782972548981E-40</v>
+      </c>
+      <c r="G7">
+        <v>220.594323404465</v>
+      </c>
+      <c r="H7">
+        <v>5.5953202920356677E-40</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>205.2353029869434</v>
+      </c>
+      <c r="B8">
+        <v>1.006360933114206E-35</v>
+      </c>
+      <c r="C8">
+        <v>207.31539051721651</v>
+      </c>
+      <c r="D8">
+        <v>5.2916250410768911E-47</v>
+      </c>
+      <c r="E8">
+        <v>157.48814473962469</v>
+      </c>
+      <c r="F8">
+        <v>4.0039149638326942E-36</v>
+      </c>
+      <c r="G8">
+        <v>205.2353029869434</v>
+      </c>
+      <c r="H8">
+        <v>1.006360933114206E-35</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="10">
+        <v>97.132160650000003</v>
+      </c>
+      <c r="B9" s="10">
+        <v>7.2387500000000003E-19</v>
+      </c>
+      <c r="C9" s="10">
+        <v>98.618877389999994</v>
+      </c>
+      <c r="D9" s="10">
+        <v>3.0608700000000003E-23</v>
+      </c>
+      <c r="E9" s="10">
+        <v>80.099272749999997</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3.5606299999999998E-19</v>
+      </c>
+      <c r="G9" s="10">
+        <v>97.132160650000003</v>
+      </c>
+      <c r="H9" s="10">
+        <v>7.2387500000000003E-19</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="10">
+        <v>58.353315899999998</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1.6373399999999999E-11</v>
+      </c>
+      <c r="C10" s="10">
+        <v>60.176857030000001</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8.6705700000000008E-15</v>
+      </c>
+      <c r="E10" s="10">
+        <v>47.01470818</v>
+      </c>
+      <c r="F10" s="10">
+        <v>7.0455999999999998E-12</v>
+      </c>
+      <c r="G10" s="10">
+        <v>58.353315899999998</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1.6373399999999999E-11</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>3800.497797563336</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3813.2226785819639</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1489.312120808579</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3800.497797563341</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>3251.5041126287751</v>
+      </c>
+      <c r="B12">
+        <v>2.5212828354348212E-283</v>
+      </c>
+      <c r="C12">
+        <v>3263.758525113557</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1299.378956122604</v>
+      </c>
+      <c r="F12">
+        <v>1.5423512247676769E-284</v>
+      </c>
+      <c r="G12">
+        <v>3251.504112628772</v>
+      </c>
+      <c r="H12">
+        <v>2.5212828354353951E-283</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>2973.7719427926149</v>
+      </c>
+      <c r="B13">
+        <v>1.8180951365129691E-253</v>
+      </c>
+      <c r="C13">
+        <v>2986.5899253046518</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1162.112061360594</v>
+      </c>
+      <c r="F13">
+        <v>1.0459606475895969E-254</v>
+      </c>
+      <c r="G13">
+        <v>2973.771942792609</v>
+      </c>
+      <c r="H13">
+        <v>1.8180951365140019E-253</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>2770.8388481098591</v>
+      </c>
+      <c r="B14">
+        <v>2.933697930455299E-226</v>
+      </c>
+      <c r="C14">
+        <v>2784.7860235198082</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1037.1618443858461</v>
+      </c>
+      <c r="F14">
+        <v>1.5023327617184401E-227</v>
+      </c>
+      <c r="G14">
+        <v>2770.8388481098659</v>
+      </c>
+      <c r="H14">
+        <v>2.933697930453298E-226</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>1931.750088300231</v>
+      </c>
+      <c r="B15">
+        <v>3.5665826560826192E-173</v>
+      </c>
+      <c r="C15">
+        <v>1943.4340606084991</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>792.48400126925844</v>
+      </c>
+      <c r="F15">
+        <v>2.3237218263490999E-174</v>
+      </c>
+      <c r="G15">
+        <v>1931.750088300231</v>
+      </c>
+      <c r="H15">
+        <v>3.5665826560826192E-173</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>1697.7091553459611</v>
+      </c>
+      <c r="B16">
+        <v>2.8203289074614798E-145</v>
+      </c>
+      <c r="C16">
+        <v>1710.5705883410069</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>664.44603221742545</v>
+      </c>
+      <c r="F16">
+        <v>1.6122647927642771E-146</v>
+      </c>
+      <c r="G16">
+        <v>1697.709155345962</v>
+      </c>
+      <c r="H16">
+        <v>2.8203289074611601E-145</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>1467.291445573821</v>
+      </c>
+      <c r="B17">
+        <v>1.001714837205352E-116</v>
+      </c>
+      <c r="C17">
+        <v>1482.1626426573389</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>533.58882998478111</v>
+      </c>
+      <c r="F17">
+        <v>4.679337060062484E-118</v>
+      </c>
+      <c r="G17">
+        <v>1467.2914455738039</v>
+      </c>
+      <c r="H17">
+        <v>1.0017148372067259E-116</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="10">
+        <v>830.06884019999995</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2.2211100000000001E-72</v>
+      </c>
+      <c r="C18" s="10">
+        <v>842.77397550000001</v>
+      </c>
+      <c r="D18" s="10">
+        <v>2.7071999999999999E-185</v>
+      </c>
+      <c r="E18" s="10">
+        <v>329.41971649999999</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1.2858E-73</v>
+      </c>
+      <c r="G18" s="10">
+        <v>830.06884019999995</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2.2211100000000001E-72</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="10">
+        <v>431.54223100000002</v>
+      </c>
+      <c r="B19" s="10">
+        <v>2.7100799999999998E-37</v>
+      </c>
+      <c r="C19" s="10">
+        <v>445.02792579999999</v>
+      </c>
+      <c r="D19" s="10">
+        <v>8.7134000000000006E-99</v>
+      </c>
+      <c r="E19" s="10">
+        <v>168.68419220000001</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1.4340299999999999E-38</v>
+      </c>
+      <c r="G19" s="10">
+        <v>431.54223100000002</v>
+      </c>
+      <c r="H19" s="10">
+        <v>2.7100799999999998E-37</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>283.72566471626391</v>
+      </c>
+      <c r="B20">
+        <v>1.620615450972563E-55</v>
+      </c>
+      <c r="C20">
+        <v>284.67563904009057</v>
+      </c>
+      <c r="D20">
+        <v>7.1899011590227289E-64</v>
+      </c>
+      <c r="E20">
+        <v>247.31201414417231</v>
+      </c>
+      <c r="F20">
+        <v>1.001053473562425E-55</v>
+      </c>
+      <c r="G20">
+        <v>283.72566471626487</v>
+      </c>
+      <c r="H20">
+        <v>1.6206154509720331E-55</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>236.98697783407181</v>
+      </c>
+      <c r="B21">
+        <v>5.2829330041048036E-47</v>
+      </c>
+      <c r="C21">
+        <v>237.88014483595899</v>
+      </c>
+      <c r="D21">
+        <v>1.140084261903774E-53</v>
+      </c>
+      <c r="E21">
+        <v>208.22793094955341</v>
+      </c>
+      <c r="F21">
+        <v>3.345712917098566E-47</v>
+      </c>
+      <c r="G21">
+        <v>236.98697783407269</v>
+      </c>
+      <c r="H21">
+        <v>5.282933004102927E-47</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>218.04372125146651</v>
+      </c>
+      <c r="B22">
+        <v>3.9924282345759009E-43</v>
+      </c>
+      <c r="C22">
+        <v>218.98356487755041</v>
+      </c>
+      <c r="D22">
+        <v>1.506941150342861E-49</v>
+      </c>
+      <c r="E22">
+        <v>190.49759278500099</v>
+      </c>
+      <c r="F22">
+        <v>2.4758140102470639E-43</v>
+      </c>
+      <c r="G22">
+        <v>218.04372125146531</v>
+      </c>
+      <c r="H22">
+        <v>3.9924282345779441E-43</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>207.03755095803169</v>
+      </c>
+      <c r="B23">
+        <v>1.6539139955599591E-40</v>
+      </c>
+      <c r="C23">
+        <v>208.07968628164599</v>
+      </c>
+      <c r="D23">
+        <v>3.6043984307667022E-47</v>
+      </c>
+      <c r="E23">
+        <v>178.5983246647211</v>
+      </c>
+      <c r="F23">
+        <v>9.8054918445844014E-41</v>
+      </c>
+      <c r="G23">
+        <v>207.03755095803231</v>
+      </c>
+      <c r="H23">
+        <v>1.6539139955596771E-40</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>139.89859863852311</v>
+      </c>
+      <c r="B24">
+        <v>1.3152041490389949E-28</v>
+      </c>
+      <c r="C24">
+        <v>140.74475951738509</v>
+      </c>
+      <c r="D24">
+        <v>1.8295952719730289E-32</v>
+      </c>
+      <c r="E24">
+        <v>123.9831307126769</v>
+      </c>
+      <c r="F24">
+        <v>8.4962860225112251E-29</v>
+      </c>
+      <c r="G24">
+        <v>139.89859863852109</v>
+      </c>
+      <c r="H24">
+        <v>1.315204149039985E-28</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>131.25224915308169</v>
+      </c>
+      <c r="B25">
+        <v>1.9299108109192441E-26</v>
+      </c>
+      <c r="C25">
+        <v>132.2465843739383</v>
+      </c>
+      <c r="D25">
+        <v>1.3214258984957501E-30</v>
+      </c>
+      <c r="E25">
+        <v>114.2196846918187</v>
+      </c>
+      <c r="F25">
+        <v>1.166427508118875E-26</v>
+      </c>
+      <c r="G25">
+        <v>131.25224915308209</v>
+      </c>
+      <c r="H25">
+        <v>1.9299108109189011E-26</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>117.7199652090565</v>
+      </c>
+      <c r="B26">
+        <v>2.593457316078204E-23</v>
+      </c>
+      <c r="C26">
+        <v>118.91307296455371</v>
+      </c>
+      <c r="D26">
+        <v>1.0942111281011661E-27</v>
+      </c>
+      <c r="E26">
+        <v>100.1141335496786</v>
+      </c>
+      <c r="F26">
+        <v>1.4386323724066031E-23</v>
+      </c>
+      <c r="G26">
+        <v>117.71996520905741</v>
+      </c>
+      <c r="H26">
+        <v>2.593457316077303E-23</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="10">
+        <v>53.943151989999997</v>
+      </c>
+      <c r="B27" s="10">
+        <v>5.4103700000000001E-12</v>
+      </c>
+      <c r="C27" s="10">
+        <v>54.76881247</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1.3557500000000001E-13</v>
+      </c>
+      <c r="E27" s="10">
+        <v>48.380649300000002</v>
+      </c>
+      <c r="F27" s="10">
+        <v>3.5101499999999999E-12</v>
+      </c>
+      <c r="G27" s="10">
+        <v>53.943151989999997</v>
+      </c>
+      <c r="H27" s="10">
+        <v>5.4103700000000001E-12</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="10">
+        <v>37.184059079999997</v>
+      </c>
+      <c r="B28" s="10">
+        <v>2.2451699999999998E-8</v>
+      </c>
+      <c r="C28" s="10">
+        <v>38.34606093</v>
+      </c>
+      <c r="D28" s="10">
+        <v>5.9247599999999997E-10</v>
+      </c>
+      <c r="E28" s="10">
+        <v>32.411004409999997</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1.24778E-8</v>
+      </c>
+      <c r="G28" s="10">
+        <v>37.184059079999997</v>
+      </c>
+      <c r="H28" s="10">
+        <v>2.2451699999999998E-8</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>6694.2422041599639</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>6716.6559615399638</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1920.873852708042</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>6694.2422041599684</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>6059.0587594877206</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>6081.8944080787542</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1720.361239330859</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>6059.0587594877125</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>5443.1932707642327</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>5466.6553107244245</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1521.7921751706331</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>5443.1932707642663</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>4633.119754730702</v>
+      </c>
+      <c r="B32">
+        <v>2.9647297719299118E-283</v>
+      </c>
+      <c r="C32">
+        <v>4656.4408273216286</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1300.882783767242</v>
+      </c>
+      <c r="F32">
+        <v>7.2674236031222947E-285</v>
+      </c>
+      <c r="G32">
+        <v>4633.1197547307247</v>
+      </c>
+      <c r="H32">
+        <v>2.9647297719262039E-283</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>4261.4172944999846</v>
+      </c>
+      <c r="B33">
+        <v>1.1726650485617781E-245</v>
+      </c>
+      <c r="C33">
+        <v>4287.1919958780099</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1128.181259741365</v>
+      </c>
+      <c r="F33">
+        <v>2.476958173115284E-247</v>
+      </c>
+      <c r="G33">
+        <v>4261.4172944999973</v>
+      </c>
+      <c r="H33">
+        <v>1.1726650485609789E-245</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>3339.9506227885231</v>
+      </c>
+      <c r="B34">
+        <v>4.3176068702939047E-195</v>
+      </c>
+      <c r="C34">
+        <v>3365.2532790217688</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>895.49300519201188</v>
+      </c>
+      <c r="F34">
+        <v>9.3667722813153151E-197</v>
+      </c>
+      <c r="G34">
+        <v>3339.950622788509</v>
+      </c>
+      <c r="H34">
+        <v>4.3176068702970948E-195</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>2467.6396169414629</v>
+      </c>
+      <c r="B35">
+        <v>1.265543865858561E-145</v>
+      </c>
+      <c r="C35">
+        <v>2492.6494779239779</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>667.94935689873273</v>
+      </c>
+      <c r="F35">
+        <v>2.7897197207503821E-147</v>
+      </c>
+      <c r="G35">
+        <v>2467.6396169414752</v>
+      </c>
+      <c r="H35">
+        <v>1.2655438658577591E-145</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="10">
+        <v>1624.3537160000001</v>
+      </c>
+      <c r="B36" s="10">
+        <v>8.4248000000000002E-97</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1649.216273</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
+        <v>443.5056189</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1.86851E-98</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1624.3537160000001</v>
+      </c>
+      <c r="H36" s="10">
+        <v>8.4248000000000002E-97</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="10">
+        <v>893.40431709999996</v>
+      </c>
+      <c r="B37" s="10">
+        <v>2.0065E-50</v>
+      </c>
+      <c r="C37" s="10">
+        <v>921.32320200000004</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2.2722999999999999E-202</v>
+      </c>
+      <c r="E37" s="10">
+        <v>230.94273219999999</v>
+      </c>
+      <c r="F37" s="10">
+        <v>3.71322E-52</v>
+      </c>
+      <c r="G37" s="10">
+        <v>893.40431709999996</v>
+      </c>
+      <c r="H37" s="10">
+        <v>2.0065E-50</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>937.36856732292756</v>
+      </c>
+      <c r="B38">
+        <v>1.8576327933484739E-141</v>
+      </c>
+      <c r="C38">
+        <v>940.50707815101782</v>
+      </c>
+      <c r="D38">
+        <v>1.5356115362360561E-206</v>
+      </c>
+      <c r="E38">
+        <v>643.65692925143048</v>
+      </c>
+      <c r="F38">
+        <v>5.3532114932885849E-142</v>
+      </c>
+      <c r="G38">
+        <v>937.36856733755883</v>
+      </c>
+      <c r="H38">
+        <v>1.8576327866998409E-141</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>727.44120975927092</v>
+      </c>
+      <c r="B39">
+        <v>2.5706335895748591E-114</v>
+      </c>
+      <c r="C39">
+        <v>730.18282235886602</v>
+      </c>
+      <c r="D39">
+        <v>8.1742184137886062E-161</v>
+      </c>
+      <c r="E39">
+        <v>518.65313049946053</v>
+      </c>
+      <c r="F39">
+        <v>8.3094429143648568E-115</v>
+      </c>
+      <c r="G39">
+        <v>727.44120975156693</v>
+      </c>
+      <c r="H39">
+        <v>2.5706335947556721E-114</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>677.15124026952344</v>
+      </c>
+      <c r="B40">
+        <v>8.6174745449531896E-105</v>
+      </c>
+      <c r="C40">
+        <v>680.06999561551277</v>
+      </c>
+      <c r="D40">
+        <v>6.452139973930866E-150</v>
+      </c>
+      <c r="E40">
+        <v>474.98021086671719</v>
+      </c>
+      <c r="F40">
+        <v>2.6427155989674789E-105</v>
+      </c>
+      <c r="G40">
+        <v>677.15124028026935</v>
+      </c>
+      <c r="H40">
+        <v>8.6174745214503441E-105</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>637.34796536950125</v>
+      </c>
+      <c r="B41">
+        <v>3.4409859482346068E-96</v>
+      </c>
+      <c r="C41">
+        <v>640.55609271196533</v>
+      </c>
+      <c r="D41">
+        <v>2.5292857725487601E-141</v>
+      </c>
+      <c r="E41">
+        <v>435.62095697831319</v>
+      </c>
+      <c r="F41">
+        <v>9.716401968057313E-97</v>
+      </c>
+      <c r="G41">
+        <v>637.34796538141643</v>
+      </c>
+      <c r="H41">
+        <v>3.4409859383127329E-96</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>445.78153827206143</v>
+      </c>
+      <c r="B42">
+        <v>4.5210813663561162E-71</v>
+      </c>
+      <c r="C42">
+        <v>448.47779757612631</v>
+      </c>
+      <c r="D42">
+        <v>1.5466433587514741E-99</v>
+      </c>
+      <c r="E42">
+        <v>319.95750673829752</v>
+      </c>
+      <c r="F42">
+        <v>1.479643854828443E-71</v>
+      </c>
+      <c r="G42">
+        <v>445.78153827363673</v>
+      </c>
+      <c r="H42">
+        <v>4.5210813644764647E-71</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>405.60156341982861</v>
+      </c>
+      <c r="B43">
+        <v>1.286890604338696E-62</v>
+      </c>
+      <c r="C43">
+        <v>408.67430253664543</v>
+      </c>
+      <c r="D43">
+        <v>7.123573104419381E-91</v>
+      </c>
+      <c r="E43">
+        <v>281.37379030985358</v>
+      </c>
+      <c r="F43">
+        <v>3.768998803723935E-63</v>
+      </c>
+      <c r="G43">
+        <v>405.60156342592501</v>
+      </c>
+      <c r="H43">
+        <v>1.2868906023961269E-62</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>356.77477888873949</v>
+      </c>
+      <c r="B44">
+        <v>9.1644448440374086E-53</v>
+      </c>
+      <c r="C44">
+        <v>360.39073948558479</v>
+      </c>
+      <c r="D44">
+        <v>2.314737181965027E-80</v>
+      </c>
+      <c r="E44">
+        <v>236.47094127632499</v>
+      </c>
+      <c r="F44">
+        <v>2.3132425130417742E-53</v>
+      </c>
+      <c r="G44">
+        <v>356.77477891285571</v>
+      </c>
+      <c r="H44">
+        <v>9.1644447937901301E-53</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="10">
+        <v>159.56525809999999</v>
+      </c>
+      <c r="B45" s="10">
+        <v>3.7809099999999999E-27</v>
+      </c>
+      <c r="C45" s="10">
+        <v>162.00758350000001</v>
+      </c>
+      <c r="D45" s="10">
+        <v>4.1212800000000003E-37</v>
+      </c>
+      <c r="E45" s="10">
+        <v>118.52323389999999</v>
+      </c>
+      <c r="F45" s="10">
+        <v>1.3318500000000001E-27</v>
+      </c>
+      <c r="G45" s="10">
+        <v>159.56525809999999</v>
+      </c>
+      <c r="H45" s="10">
+        <v>3.7809099999999999E-27</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="10">
+        <v>164.90973389999999</v>
+      </c>
+      <c r="B46" s="10">
+        <v>1.4596099999999999E-22</v>
+      </c>
+      <c r="C46" s="10">
+        <v>170.0631631</v>
+      </c>
+      <c r="D46" s="10">
+        <v>7.1675599999999998E-39</v>
+      </c>
+      <c r="E46" s="10">
+        <v>98.982804599999994</v>
+      </c>
+      <c r="F46" s="10">
+        <v>2.54704E-23</v>
+      </c>
+      <c r="G46" s="10">
+        <v>164.90973389999999</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1.4596099999999999E-22</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47">
+        <v>2299.9347980379011</v>
+      </c>
+      <c r="B47">
+        <v>1.177720707789261E-249</v>
+      </c>
+      <c r="C47">
+        <v>2307.6354725849028</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1143.2533488371321</v>
+      </c>
+      <c r="F47">
+        <v>1.3127419471683399E-250</v>
+      </c>
+      <c r="G47">
+        <v>2299.9347980379289</v>
+      </c>
+      <c r="H47">
+        <v>1.1777207077845741E-249</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>1892.5932554936719</v>
+      </c>
+      <c r="B48">
+        <v>1.379626963300126E-212</v>
+      </c>
+      <c r="C48">
+        <v>1899.7261446475429</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>972.52218309588898</v>
+      </c>
+      <c r="F48">
+        <v>1.6866930555828251E-213</v>
+      </c>
+      <c r="G48">
+        <v>1892.5932554936931</v>
+      </c>
+      <c r="H48">
+        <v>1.3796269632959699E-212</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49">
+        <v>1717.6192763509939</v>
+      </c>
+      <c r="B49">
+        <v>4.1056653542523022E-190</v>
+      </c>
+      <c r="C49">
+        <v>1725.0228077145759</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>869.22957680997933</v>
+      </c>
+      <c r="F49">
+        <v>4.7981105866297619E-191</v>
+      </c>
+      <c r="G49">
+        <v>1717.6192763509871</v>
+      </c>
+      <c r="H49">
+        <v>4.1056653542560359E-190</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50">
+        <v>1508.864594183422</v>
+      </c>
+      <c r="B50">
+        <v>1.9441069909753859E-165</v>
+      </c>
+      <c r="C50">
+        <v>1516.459550194412</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>755.79768495594362</v>
+      </c>
+      <c r="F50">
+        <v>2.2018237302964771E-166</v>
+      </c>
+      <c r="G50">
+        <v>1508.8645941834079</v>
+      </c>
+      <c r="H50">
+        <v>1.9441069909790331E-165</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51">
+        <v>1166.9360362866721</v>
+      </c>
+      <c r="B51">
+        <v>2.152015368146386E-132</v>
+      </c>
+      <c r="C51">
+        <v>1173.994117151309</v>
+      </c>
+      <c r="D51">
+        <v>2.7362421192766769E-257</v>
+      </c>
+      <c r="E51">
+        <v>603.67228035213157</v>
+      </c>
+      <c r="F51">
+        <v>2.661048936562501E-133</v>
+      </c>
+      <c r="G51">
+        <v>1166.936036286671</v>
+      </c>
+      <c r="H51">
+        <v>2.1520153681466309E-132</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52">
+        <v>970.83598632631174</v>
+      </c>
+      <c r="B52">
+        <v>1.407532157930548E-108</v>
+      </c>
+      <c r="C52">
+        <v>978.19080440454138</v>
+      </c>
+      <c r="D52">
+        <v>9.8821427841834187E-215</v>
+      </c>
+      <c r="E52">
+        <v>494.29701537433539</v>
+      </c>
+      <c r="F52">
+        <v>1.6551553338131309E-109</v>
+      </c>
+      <c r="G52">
+        <v>970.83598632629469</v>
+      </c>
+      <c r="H52">
+        <v>1.4075321579340281E-108</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53">
+        <v>879.5978807580874</v>
+      </c>
+      <c r="B53">
+        <v>1.205861146145225E-90</v>
+      </c>
+      <c r="C53">
+        <v>888.51272414414927</v>
+      </c>
+      <c r="D53">
+        <v>3.083430876335398E-195</v>
+      </c>
+      <c r="E53">
+        <v>412.37263058130878</v>
+      </c>
+      <c r="F53">
+        <v>1.1160131696486921E-91</v>
+      </c>
+      <c r="G53">
+        <v>879.5978807580849</v>
+      </c>
+      <c r="H53">
+        <v>1.20586114614558E-90</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="10">
+        <v>435.97504409999999</v>
+      </c>
+      <c r="B54" s="10">
+        <v>1.01718E-51</v>
+      </c>
+      <c r="C54" s="10">
+        <v>442.6481316</v>
+      </c>
+      <c r="D54" s="10">
+        <v>2.8715399999999999E-98</v>
+      </c>
+      <c r="E54" s="10">
+        <v>232.97631419999999</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1.3374399999999999E-52</v>
+      </c>
+      <c r="G54" s="10">
+        <v>435.97504409999999</v>
+      </c>
+      <c r="H54" s="10">
+        <v>1.01718E-51</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="10">
+        <v>261.11707919999998</v>
+      </c>
+      <c r="B55" s="10">
+        <v>3.8918499999999997E-29</v>
+      </c>
+      <c r="C55" s="10">
+        <v>269.27698789999999</v>
+      </c>
+      <c r="D55" s="10">
+        <v>1.6311299999999999E-60</v>
+      </c>
+      <c r="E55" s="10">
+        <v>130.05783349999999</v>
+      </c>
+      <c r="F55" s="10">
+        <v>3.98011E-30</v>
+      </c>
+      <c r="G55" s="10">
+        <v>261.11707919999998</v>
+      </c>
+      <c r="H55" s="10">
+        <v>3.8918499999999997E-29</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>